<commit_message>
Tests for adj and targets created
</commit_message>
<xml_diff>
--- a/resources/clueLayout.xlsx
+++ b/resources/clueLayout.xlsx
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +147,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +214,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -358,12 +396,41 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC0C0C0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -662,7 +729,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +777,7 @@
       <c r="L1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="22" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="5" t="s">
@@ -781,7 +848,7 @@
       <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="22" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -858,13 +925,13 @@
       <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="18" t="s">
         <v>18</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="22" t="s">
         <v>18</v>
       </c>
       <c r="P3" s="5" t="s">
@@ -929,7 +996,7 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="22" t="s">
         <v>18</v>
       </c>
       <c r="M4" s="5" t="s">
@@ -973,7 +1040,7 @@
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1056,7 +1123,7 @@
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1127,13 +1194,13 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1160,7 +1227,7 @@
       <c r="N7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="25" t="s">
         <v>18</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -1198,7 +1265,7 @@
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1210,7 +1277,7 @@
       <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1231,13 +1298,13 @@
       <c r="M8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="25" t="s">
         <v>18</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="25" t="s">
         <v>18</v>
       </c>
       <c r="Q8" s="1" t="s">
@@ -1272,16 +1339,16 @@
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1308,7 +1375,7 @@
       <c r="N9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="25" t="s">
         <v>18</v>
       </c>
       <c r="P9" s="5" t="s">
@@ -1352,7 +1419,7 @@
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1379,13 +1446,13 @@
       <c r="M10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="25" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5" t="s">
@@ -1462,7 +1529,7 @@
       <c r="N11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="25" t="s">
         <v>18</v>
       </c>
       <c r="P11" s="5" t="s">
@@ -1509,7 +1576,7 @@
       <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1539,13 +1606,13 @@
       <c r="M12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="25" t="s">
         <v>18</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="25" t="s">
         <v>18</v>
       </c>
       <c r="Q12" s="1" t="s">
@@ -1622,7 +1689,7 @@
       <c r="N13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="25" t="s">
         <v>18</v>
       </c>
       <c r="P13" s="1" t="s">
@@ -1714,7 +1781,7 @@
       <c r="R14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S14" s="16" t="s">
+      <c r="S14" s="21" t="s">
         <v>18</v>
       </c>
       <c r="T14" s="1" t="s">
@@ -1791,13 +1858,13 @@
       <c r="Q15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="R15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="T15" s="22" t="s">
         <v>18</v>
       </c>
       <c r="U15" s="1" t="s">
@@ -1853,7 +1920,7 @@
       <c r="K16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="23" t="s">
         <v>25</v>
       </c>
       <c r="M16" s="1" t="s">
@@ -1868,19 +1935,19 @@
       <c r="P16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="22" t="s">
         <v>18</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="18" t="s">
         <v>18</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="U16" s="22" t="s">
         <v>18</v>
       </c>
       <c r="V16" s="1" t="s">
@@ -1930,13 +1997,13 @@
       <c r="J17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="22" t="s">
         <v>18</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M17" s="22" t="s">
         <v>18</v>
       </c>
       <c r="N17" s="1" t="s">
@@ -1951,10 +2018,10 @@
       <c r="Q17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R17" s="12" t="s">
+      <c r="R17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="S17" s="12" t="s">
+      <c r="S17" s="23" t="s">
         <v>24</v>
       </c>
       <c r="T17" s="5" t="s">
@@ -2007,19 +2074,19 @@
       <c r="I18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="22" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="22" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" s="22" t="s">
         <v>18</v>
       </c>
       <c r="O18" s="5" t="s">
@@ -2084,19 +2151,19 @@
       <c r="H19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="22" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="22" t="s">
         <v>18</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="22" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="1" t="s">
@@ -2152,7 +2219,7 @@
       <c r="D20" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="13" t="s">
@@ -2167,19 +2234,19 @@
       <c r="I20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="22" t="s">
         <v>18</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="18" t="s">
         <v>18</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="N20" s="22" t="s">
         <v>18</v>
       </c>
       <c r="O20" s="5" t="s">
@@ -2247,16 +2314,16 @@
       <c r="I21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" s="22" t="s">
         <v>18</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M21" s="22" t="s">
         <v>18</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -2327,13 +2394,13 @@
       <c r="K22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="22" t="s">
         <v>18</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="N22" s="22" t="s">
         <v>18</v>
       </c>
       <c r="O22" s="1" t="s">

</xml_diff>